<commit_message>
[IMP] Adjust Receivable Before Due
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_before_due.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_before_due.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Receivable Balance (Before Due) Report</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">Report Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due Date</t>
   </si>
   <si>
     <t xml:space="preserve">System Origin</t>
@@ -246,10 +249,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -257,9 +260,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5510204081633"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.3112244897959"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="27"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="27.2397959183673"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="26.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.3112244897959"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="21.2397959183673"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="4" width="23.6428571428571"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="5" width="25.5561224489796"/>
@@ -4318,7 +4321,10 @@
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="11" t="n">
+        <f aca="false">B4+B3</f>
+        <v>0</v>
+      </c>
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
       <c r="E5" s="4"/>
@@ -6342,7 +6348,7 @@
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="4"/>
@@ -7351,8 +7357,10 @@
       <c r="ALT7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="4"/>
@@ -8360,56 +8368,1066 @@
       <c r="ALS8" s="0"/>
       <c r="ALT8" s="0"/>
     </row>
-    <row r="9" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="12" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
+      <c r="AJ9" s="0"/>
+      <c r="AK9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AM9" s="0"/>
+      <c r="AN9" s="0"/>
+      <c r="AO9" s="0"/>
+      <c r="AP9" s="0"/>
+      <c r="AQ9" s="0"/>
+      <c r="AR9" s="0"/>
+      <c r="AS9" s="0"/>
+      <c r="AT9" s="0"/>
+      <c r="AU9" s="0"/>
+      <c r="AV9" s="0"/>
+      <c r="AW9" s="0"/>
+      <c r="AX9" s="0"/>
+      <c r="AY9" s="0"/>
+      <c r="AZ9" s="0"/>
+      <c r="BA9" s="0"/>
+      <c r="BB9" s="0"/>
+      <c r="BC9" s="0"/>
+      <c r="BD9" s="0"/>
+      <c r="BE9" s="0"/>
+      <c r="BF9" s="0"/>
+      <c r="BG9" s="0"/>
+      <c r="BH9" s="0"/>
+      <c r="BI9" s="0"/>
+      <c r="BJ9" s="0"/>
+      <c r="BK9" s="0"/>
+      <c r="BL9" s="0"/>
+      <c r="BM9" s="0"/>
+      <c r="BN9" s="0"/>
+      <c r="BO9" s="0"/>
+      <c r="BP9" s="0"/>
+      <c r="BQ9" s="0"/>
+      <c r="BR9" s="0"/>
+      <c r="BS9" s="0"/>
+      <c r="BT9" s="0"/>
+      <c r="BU9" s="0"/>
+      <c r="BV9" s="0"/>
+      <c r="BW9" s="0"/>
+      <c r="BX9" s="0"/>
+      <c r="BY9" s="0"/>
+      <c r="BZ9" s="0"/>
+      <c r="CA9" s="0"/>
+      <c r="CB9" s="0"/>
+      <c r="CC9" s="0"/>
+      <c r="CD9" s="0"/>
+      <c r="CE9" s="0"/>
+      <c r="CF9" s="0"/>
+      <c r="CG9" s="0"/>
+      <c r="CH9" s="0"/>
+      <c r="CI9" s="0"/>
+      <c r="CJ9" s="0"/>
+      <c r="CK9" s="0"/>
+      <c r="CL9" s="0"/>
+      <c r="CM9" s="0"/>
+      <c r="CN9" s="0"/>
+      <c r="CO9" s="0"/>
+      <c r="CP9" s="0"/>
+      <c r="CQ9" s="0"/>
+      <c r="CR9" s="0"/>
+      <c r="CS9" s="0"/>
+      <c r="CT9" s="0"/>
+      <c r="CU9" s="0"/>
+      <c r="CV9" s="0"/>
+      <c r="CW9" s="0"/>
+      <c r="CX9" s="0"/>
+      <c r="CY9" s="0"/>
+      <c r="CZ9" s="0"/>
+      <c r="DA9" s="0"/>
+      <c r="DB9" s="0"/>
+      <c r="DC9" s="0"/>
+      <c r="DD9" s="0"/>
+      <c r="DE9" s="0"/>
+      <c r="DF9" s="0"/>
+      <c r="DG9" s="0"/>
+      <c r="DH9" s="0"/>
+      <c r="DI9" s="0"/>
+      <c r="DJ9" s="0"/>
+      <c r="DK9" s="0"/>
+      <c r="DL9" s="0"/>
+      <c r="DM9" s="0"/>
+      <c r="DN9" s="0"/>
+      <c r="DO9" s="0"/>
+      <c r="DP9" s="0"/>
+      <c r="DQ9" s="0"/>
+      <c r="DR9" s="0"/>
+      <c r="DS9" s="0"/>
+      <c r="DT9" s="0"/>
+      <c r="DU9" s="0"/>
+      <c r="DV9" s="0"/>
+      <c r="DW9" s="0"/>
+      <c r="DX9" s="0"/>
+      <c r="DY9" s="0"/>
+      <c r="DZ9" s="0"/>
+      <c r="EA9" s="0"/>
+      <c r="EB9" s="0"/>
+      <c r="EC9" s="0"/>
+      <c r="ED9" s="0"/>
+      <c r="EE9" s="0"/>
+      <c r="EF9" s="0"/>
+      <c r="EG9" s="0"/>
+      <c r="EH9" s="0"/>
+      <c r="EI9" s="0"/>
+      <c r="EJ9" s="0"/>
+      <c r="EK9" s="0"/>
+      <c r="EL9" s="0"/>
+      <c r="EM9" s="0"/>
+      <c r="EN9" s="0"/>
+      <c r="EO9" s="0"/>
+      <c r="EP9" s="0"/>
+      <c r="EQ9" s="0"/>
+      <c r="ER9" s="0"/>
+      <c r="ES9" s="0"/>
+      <c r="ET9" s="0"/>
+      <c r="EU9" s="0"/>
+      <c r="EV9" s="0"/>
+      <c r="EW9" s="0"/>
+      <c r="EX9" s="0"/>
+      <c r="EY9" s="0"/>
+      <c r="EZ9" s="0"/>
+      <c r="FA9" s="0"/>
+      <c r="FB9" s="0"/>
+      <c r="FC9" s="0"/>
+      <c r="FD9" s="0"/>
+      <c r="FE9" s="0"/>
+      <c r="FF9" s="0"/>
+      <c r="FG9" s="0"/>
+      <c r="FH9" s="0"/>
+      <c r="FI9" s="0"/>
+      <c r="FJ9" s="0"/>
+      <c r="FK9" s="0"/>
+      <c r="FL9" s="0"/>
+      <c r="FM9" s="0"/>
+      <c r="FN9" s="0"/>
+      <c r="FO9" s="0"/>
+      <c r="FP9" s="0"/>
+      <c r="FQ9" s="0"/>
+      <c r="FR9" s="0"/>
+      <c r="FS9" s="0"/>
+      <c r="FT9" s="0"/>
+      <c r="FU9" s="0"/>
+      <c r="FV9" s="0"/>
+      <c r="FW9" s="0"/>
+      <c r="FX9" s="0"/>
+      <c r="FY9" s="0"/>
+      <c r="FZ9" s="0"/>
+      <c r="GA9" s="0"/>
+      <c r="GB9" s="0"/>
+      <c r="GC9" s="0"/>
+      <c r="GD9" s="0"/>
+      <c r="GE9" s="0"/>
+      <c r="GF9" s="0"/>
+      <c r="GG9" s="0"/>
+      <c r="GH9" s="0"/>
+      <c r="GI9" s="0"/>
+      <c r="GJ9" s="0"/>
+      <c r="GK9" s="0"/>
+      <c r="GL9" s="0"/>
+      <c r="GM9" s="0"/>
+      <c r="GN9" s="0"/>
+      <c r="GO9" s="0"/>
+      <c r="GP9" s="0"/>
+      <c r="GQ9" s="0"/>
+      <c r="GR9" s="0"/>
+      <c r="GS9" s="0"/>
+      <c r="GT9" s="0"/>
+      <c r="GU9" s="0"/>
+      <c r="GV9" s="0"/>
+      <c r="GW9" s="0"/>
+      <c r="GX9" s="0"/>
+      <c r="GY9" s="0"/>
+      <c r="GZ9" s="0"/>
+      <c r="HA9" s="0"/>
+      <c r="HB9" s="0"/>
+      <c r="HC9" s="0"/>
+      <c r="HD9" s="0"/>
+      <c r="HE9" s="0"/>
+      <c r="HF9" s="0"/>
+      <c r="HG9" s="0"/>
+      <c r="HH9" s="0"/>
+      <c r="HI9" s="0"/>
+      <c r="HJ9" s="0"/>
+      <c r="HK9" s="0"/>
+      <c r="HL9" s="0"/>
+      <c r="HM9" s="0"/>
+      <c r="HN9" s="0"/>
+      <c r="HO9" s="0"/>
+      <c r="HP9" s="0"/>
+      <c r="HQ9" s="0"/>
+      <c r="HR9" s="0"/>
+      <c r="HS9" s="0"/>
+      <c r="HT9" s="0"/>
+      <c r="HU9" s="0"/>
+      <c r="HV9" s="0"/>
+      <c r="HW9" s="0"/>
+      <c r="HX9" s="0"/>
+      <c r="HY9" s="0"/>
+      <c r="HZ9" s="0"/>
+      <c r="IA9" s="0"/>
+      <c r="IB9" s="0"/>
+      <c r="IC9" s="0"/>
+      <c r="ID9" s="0"/>
+      <c r="IE9" s="0"/>
+      <c r="IF9" s="0"/>
+      <c r="IG9" s="0"/>
+      <c r="IH9" s="0"/>
+      <c r="II9" s="0"/>
+      <c r="IJ9" s="0"/>
+      <c r="IK9" s="0"/>
+      <c r="IL9" s="0"/>
+      <c r="IM9" s="0"/>
+      <c r="IN9" s="0"/>
+      <c r="IO9" s="0"/>
+      <c r="IP9" s="0"/>
+      <c r="IQ9" s="0"/>
+      <c r="IR9" s="0"/>
+      <c r="IS9" s="0"/>
+      <c r="IT9" s="0"/>
+      <c r="IU9" s="0"/>
+      <c r="IV9" s="0"/>
+      <c r="IW9" s="0"/>
+      <c r="IX9" s="0"/>
+      <c r="IY9" s="0"/>
+      <c r="IZ9" s="0"/>
+      <c r="JA9" s="0"/>
+      <c r="JB9" s="0"/>
+      <c r="JC9" s="0"/>
+      <c r="JD9" s="0"/>
+      <c r="JE9" s="0"/>
+      <c r="JF9" s="0"/>
+      <c r="JG9" s="0"/>
+      <c r="JH9" s="0"/>
+      <c r="JI9" s="0"/>
+      <c r="JJ9" s="0"/>
+      <c r="JK9" s="0"/>
+      <c r="JL9" s="0"/>
+      <c r="JM9" s="0"/>
+      <c r="JN9" s="0"/>
+      <c r="JO9" s="0"/>
+      <c r="JP9" s="0"/>
+      <c r="JQ9" s="0"/>
+      <c r="JR9" s="0"/>
+      <c r="JS9" s="0"/>
+      <c r="JT9" s="0"/>
+      <c r="JU9" s="0"/>
+      <c r="JV9" s="0"/>
+      <c r="JW9" s="0"/>
+      <c r="JX9" s="0"/>
+      <c r="JY9" s="0"/>
+      <c r="JZ9" s="0"/>
+      <c r="KA9" s="0"/>
+      <c r="KB9" s="0"/>
+      <c r="KC9" s="0"/>
+      <c r="KD9" s="0"/>
+      <c r="KE9" s="0"/>
+      <c r="KF9" s="0"/>
+      <c r="KG9" s="0"/>
+      <c r="KH9" s="0"/>
+      <c r="KI9" s="0"/>
+      <c r="KJ9" s="0"/>
+      <c r="KK9" s="0"/>
+      <c r="KL9" s="0"/>
+      <c r="KM9" s="0"/>
+      <c r="KN9" s="0"/>
+      <c r="KO9" s="0"/>
+      <c r="KP9" s="0"/>
+      <c r="KQ9" s="0"/>
+      <c r="KR9" s="0"/>
+      <c r="KS9" s="0"/>
+      <c r="KT9" s="0"/>
+      <c r="KU9" s="0"/>
+      <c r="KV9" s="0"/>
+      <c r="KW9" s="0"/>
+      <c r="KX9" s="0"/>
+      <c r="KY9" s="0"/>
+      <c r="KZ9" s="0"/>
+      <c r="LA9" s="0"/>
+      <c r="LB9" s="0"/>
+      <c r="LC9" s="0"/>
+      <c r="LD9" s="0"/>
+      <c r="LE9" s="0"/>
+      <c r="LF9" s="0"/>
+      <c r="LG9" s="0"/>
+      <c r="LH9" s="0"/>
+      <c r="LI9" s="0"/>
+      <c r="LJ9" s="0"/>
+      <c r="LK9" s="0"/>
+      <c r="LL9" s="0"/>
+      <c r="LM9" s="0"/>
+      <c r="LN9" s="0"/>
+      <c r="LO9" s="0"/>
+      <c r="LP9" s="0"/>
+      <c r="LQ9" s="0"/>
+      <c r="LR9" s="0"/>
+      <c r="LS9" s="0"/>
+      <c r="LT9" s="0"/>
+      <c r="LU9" s="0"/>
+      <c r="LV9" s="0"/>
+      <c r="LW9" s="0"/>
+      <c r="LX9" s="0"/>
+      <c r="LY9" s="0"/>
+      <c r="LZ9" s="0"/>
+      <c r="MA9" s="0"/>
+      <c r="MB9" s="0"/>
+      <c r="MC9" s="0"/>
+      <c r="MD9" s="0"/>
+      <c r="ME9" s="0"/>
+      <c r="MF9" s="0"/>
+      <c r="MG9" s="0"/>
+      <c r="MH9" s="0"/>
+      <c r="MI9" s="0"/>
+      <c r="MJ9" s="0"/>
+      <c r="MK9" s="0"/>
+      <c r="ML9" s="0"/>
+      <c r="MM9" s="0"/>
+      <c r="MN9" s="0"/>
+      <c r="MO9" s="0"/>
+      <c r="MP9" s="0"/>
+      <c r="MQ9" s="0"/>
+      <c r="MR9" s="0"/>
+      <c r="MS9" s="0"/>
+      <c r="MT9" s="0"/>
+      <c r="MU9" s="0"/>
+      <c r="MV9" s="0"/>
+      <c r="MW9" s="0"/>
+      <c r="MX9" s="0"/>
+      <c r="MY9" s="0"/>
+      <c r="MZ9" s="0"/>
+      <c r="NA9" s="0"/>
+      <c r="NB9" s="0"/>
+      <c r="NC9" s="0"/>
+      <c r="ND9" s="0"/>
+      <c r="NE9" s="0"/>
+      <c r="NF9" s="0"/>
+      <c r="NG9" s="0"/>
+      <c r="NH9" s="0"/>
+      <c r="NI9" s="0"/>
+      <c r="NJ9" s="0"/>
+      <c r="NK9" s="0"/>
+      <c r="NL9" s="0"/>
+      <c r="NM9" s="0"/>
+      <c r="NN9" s="0"/>
+      <c r="NO9" s="0"/>
+      <c r="NP9" s="0"/>
+      <c r="NQ9" s="0"/>
+      <c r="NR9" s="0"/>
+      <c r="NS9" s="0"/>
+      <c r="NT9" s="0"/>
+      <c r="NU9" s="0"/>
+      <c r="NV9" s="0"/>
+      <c r="NW9" s="0"/>
+      <c r="NX9" s="0"/>
+      <c r="NY9" s="0"/>
+      <c r="NZ9" s="0"/>
+      <c r="OA9" s="0"/>
+      <c r="OB9" s="0"/>
+      <c r="OC9" s="0"/>
+      <c r="OD9" s="0"/>
+      <c r="OE9" s="0"/>
+      <c r="OF9" s="0"/>
+      <c r="OG9" s="0"/>
+      <c r="OH9" s="0"/>
+      <c r="OI9" s="0"/>
+      <c r="OJ9" s="0"/>
+      <c r="OK9" s="0"/>
+      <c r="OL9" s="0"/>
+      <c r="OM9" s="0"/>
+      <c r="ON9" s="0"/>
+      <c r="OO9" s="0"/>
+      <c r="OP9" s="0"/>
+      <c r="OQ9" s="0"/>
+      <c r="OR9" s="0"/>
+      <c r="OS9" s="0"/>
+      <c r="OT9" s="0"/>
+      <c r="OU9" s="0"/>
+      <c r="OV9" s="0"/>
+      <c r="OW9" s="0"/>
+      <c r="OX9" s="0"/>
+      <c r="OY9" s="0"/>
+      <c r="OZ9" s="0"/>
+      <c r="PA9" s="0"/>
+      <c r="PB9" s="0"/>
+      <c r="PC9" s="0"/>
+      <c r="PD9" s="0"/>
+      <c r="PE9" s="0"/>
+      <c r="PF9" s="0"/>
+      <c r="PG9" s="0"/>
+      <c r="PH9" s="0"/>
+      <c r="PI9" s="0"/>
+      <c r="PJ9" s="0"/>
+      <c r="PK9" s="0"/>
+      <c r="PL9" s="0"/>
+      <c r="PM9" s="0"/>
+      <c r="PN9" s="0"/>
+      <c r="PO9" s="0"/>
+      <c r="PP9" s="0"/>
+      <c r="PQ9" s="0"/>
+      <c r="PR9" s="0"/>
+      <c r="PS9" s="0"/>
+      <c r="PT9" s="0"/>
+      <c r="PU9" s="0"/>
+      <c r="PV9" s="0"/>
+      <c r="PW9" s="0"/>
+      <c r="PX9" s="0"/>
+      <c r="PY9" s="0"/>
+      <c r="PZ9" s="0"/>
+      <c r="QA9" s="0"/>
+      <c r="QB9" s="0"/>
+      <c r="QC9" s="0"/>
+      <c r="QD9" s="0"/>
+      <c r="QE9" s="0"/>
+      <c r="QF9" s="0"/>
+      <c r="QG9" s="0"/>
+      <c r="QH9" s="0"/>
+      <c r="QI9" s="0"/>
+      <c r="QJ9" s="0"/>
+      <c r="QK9" s="0"/>
+      <c r="QL9" s="0"/>
+      <c r="QM9" s="0"/>
+      <c r="QN9" s="0"/>
+      <c r="QO9" s="0"/>
+      <c r="QP9" s="0"/>
+      <c r="QQ9" s="0"/>
+      <c r="QR9" s="0"/>
+      <c r="QS9" s="0"/>
+      <c r="QT9" s="0"/>
+      <c r="QU9" s="0"/>
+      <c r="QV9" s="0"/>
+      <c r="QW9" s="0"/>
+      <c r="QX9" s="0"/>
+      <c r="QY9" s="0"/>
+      <c r="QZ9" s="0"/>
+      <c r="RA9" s="0"/>
+      <c r="RB9" s="0"/>
+      <c r="RC9" s="0"/>
+      <c r="RD9" s="0"/>
+      <c r="RE9" s="0"/>
+      <c r="RF9" s="0"/>
+      <c r="RG9" s="0"/>
+      <c r="RH9" s="0"/>
+      <c r="RI9" s="0"/>
+      <c r="RJ9" s="0"/>
+      <c r="RK9" s="0"/>
+      <c r="RL9" s="0"/>
+      <c r="RM9" s="0"/>
+      <c r="RN9" s="0"/>
+      <c r="RO9" s="0"/>
+      <c r="RP9" s="0"/>
+      <c r="RQ9" s="0"/>
+      <c r="RR9" s="0"/>
+      <c r="RS9" s="0"/>
+      <c r="RT9" s="0"/>
+      <c r="RU9" s="0"/>
+      <c r="RV9" s="0"/>
+      <c r="RW9" s="0"/>
+      <c r="RX9" s="0"/>
+      <c r="RY9" s="0"/>
+      <c r="RZ9" s="0"/>
+      <c r="SA9" s="0"/>
+      <c r="SB9" s="0"/>
+      <c r="SC9" s="0"/>
+      <c r="SD9" s="0"/>
+      <c r="SE9" s="0"/>
+      <c r="SF9" s="0"/>
+      <c r="SG9" s="0"/>
+      <c r="SH9" s="0"/>
+      <c r="SI9" s="0"/>
+      <c r="SJ9" s="0"/>
+      <c r="SK9" s="0"/>
+      <c r="SL9" s="0"/>
+      <c r="SM9" s="0"/>
+      <c r="SN9" s="0"/>
+      <c r="SO9" s="0"/>
+      <c r="SP9" s="0"/>
+      <c r="SQ9" s="0"/>
+      <c r="SR9" s="0"/>
+      <c r="SS9" s="0"/>
+      <c r="ST9" s="0"/>
+      <c r="SU9" s="0"/>
+      <c r="SV9" s="0"/>
+      <c r="SW9" s="0"/>
+      <c r="SX9" s="0"/>
+      <c r="SY9" s="0"/>
+      <c r="SZ9" s="0"/>
+      <c r="TA9" s="0"/>
+      <c r="TB9" s="0"/>
+      <c r="TC9" s="0"/>
+      <c r="TD9" s="0"/>
+      <c r="TE9" s="0"/>
+      <c r="TF9" s="0"/>
+      <c r="TG9" s="0"/>
+      <c r="TH9" s="0"/>
+      <c r="TI9" s="0"/>
+      <c r="TJ9" s="0"/>
+      <c r="TK9" s="0"/>
+      <c r="TL9" s="0"/>
+      <c r="TM9" s="0"/>
+      <c r="TN9" s="0"/>
+      <c r="TO9" s="0"/>
+      <c r="TP9" s="0"/>
+      <c r="TQ9" s="0"/>
+      <c r="TR9" s="0"/>
+      <c r="TS9" s="0"/>
+      <c r="TT9" s="0"/>
+      <c r="TU9" s="0"/>
+      <c r="TV9" s="0"/>
+      <c r="TW9" s="0"/>
+      <c r="TX9" s="0"/>
+      <c r="TY9" s="0"/>
+      <c r="TZ9" s="0"/>
+      <c r="UA9" s="0"/>
+      <c r="UB9" s="0"/>
+      <c r="UC9" s="0"/>
+      <c r="UD9" s="0"/>
+      <c r="UE9" s="0"/>
+      <c r="UF9" s="0"/>
+      <c r="UG9" s="0"/>
+      <c r="UH9" s="0"/>
+      <c r="UI9" s="0"/>
+      <c r="UJ9" s="0"/>
+      <c r="UK9" s="0"/>
+      <c r="UL9" s="0"/>
+      <c r="UM9" s="0"/>
+      <c r="UN9" s="0"/>
+      <c r="UO9" s="0"/>
+      <c r="UP9" s="0"/>
+      <c r="UQ9" s="0"/>
+      <c r="UR9" s="0"/>
+      <c r="US9" s="0"/>
+      <c r="UT9" s="0"/>
+      <c r="UU9" s="0"/>
+      <c r="UV9" s="0"/>
+      <c r="UW9" s="0"/>
+      <c r="UX9" s="0"/>
+      <c r="UY9" s="0"/>
+      <c r="UZ9" s="0"/>
+      <c r="VA9" s="0"/>
+      <c r="VB9" s="0"/>
+      <c r="VC9" s="0"/>
+      <c r="VD9" s="0"/>
+      <c r="VE9" s="0"/>
+      <c r="VF9" s="0"/>
+      <c r="VG9" s="0"/>
+      <c r="VH9" s="0"/>
+      <c r="VI9" s="0"/>
+      <c r="VJ9" s="0"/>
+      <c r="VK9" s="0"/>
+      <c r="VL9" s="0"/>
+      <c r="VM9" s="0"/>
+      <c r="VN9" s="0"/>
+      <c r="VO9" s="0"/>
+      <c r="VP9" s="0"/>
+      <c r="VQ9" s="0"/>
+      <c r="VR9" s="0"/>
+      <c r="VS9" s="0"/>
+      <c r="VT9" s="0"/>
+      <c r="VU9" s="0"/>
+      <c r="VV9" s="0"/>
+      <c r="VW9" s="0"/>
+      <c r="VX9" s="0"/>
+      <c r="VY9" s="0"/>
+      <c r="VZ9" s="0"/>
+      <c r="WA9" s="0"/>
+      <c r="WB9" s="0"/>
+      <c r="WC9" s="0"/>
+      <c r="WD9" s="0"/>
+      <c r="WE9" s="0"/>
+      <c r="WF9" s="0"/>
+      <c r="WG9" s="0"/>
+      <c r="WH9" s="0"/>
+      <c r="WI9" s="0"/>
+      <c r="WJ9" s="0"/>
+      <c r="WK9" s="0"/>
+      <c r="WL9" s="0"/>
+      <c r="WM9" s="0"/>
+      <c r="WN9" s="0"/>
+      <c r="WO9" s="0"/>
+      <c r="WP9" s="0"/>
+      <c r="WQ9" s="0"/>
+      <c r="WR9" s="0"/>
+      <c r="WS9" s="0"/>
+      <c r="WT9" s="0"/>
+      <c r="WU9" s="0"/>
+      <c r="WV9" s="0"/>
+      <c r="WW9" s="0"/>
+      <c r="WX9" s="0"/>
+      <c r="WY9" s="0"/>
+      <c r="WZ9" s="0"/>
+      <c r="XA9" s="0"/>
+      <c r="XB9" s="0"/>
+      <c r="XC9" s="0"/>
+      <c r="XD9" s="0"/>
+      <c r="XE9" s="0"/>
+      <c r="XF9" s="0"/>
+      <c r="XG9" s="0"/>
+      <c r="XH9" s="0"/>
+      <c r="XI9" s="0"/>
+      <c r="XJ9" s="0"/>
+      <c r="XK9" s="0"/>
+      <c r="XL9" s="0"/>
+      <c r="XM9" s="0"/>
+      <c r="XN9" s="0"/>
+      <c r="XO9" s="0"/>
+      <c r="XP9" s="0"/>
+      <c r="XQ9" s="0"/>
+      <c r="XR9" s="0"/>
+      <c r="XS9" s="0"/>
+      <c r="XT9" s="0"/>
+      <c r="XU9" s="0"/>
+      <c r="XV9" s="0"/>
+      <c r="XW9" s="0"/>
+      <c r="XX9" s="0"/>
+      <c r="XY9" s="0"/>
+      <c r="XZ9" s="0"/>
+      <c r="YA9" s="0"/>
+      <c r="YB9" s="0"/>
+      <c r="YC9" s="0"/>
+      <c r="YD9" s="0"/>
+      <c r="YE9" s="0"/>
+      <c r="YF9" s="0"/>
+      <c r="YG9" s="0"/>
+      <c r="YH9" s="0"/>
+      <c r="YI9" s="0"/>
+      <c r="YJ9" s="0"/>
+      <c r="YK9" s="0"/>
+      <c r="YL9" s="0"/>
+      <c r="YM9" s="0"/>
+      <c r="YN9" s="0"/>
+      <c r="YO9" s="0"/>
+      <c r="YP9" s="0"/>
+      <c r="YQ9" s="0"/>
+      <c r="YR9" s="0"/>
+      <c r="YS9" s="0"/>
+      <c r="YT9" s="0"/>
+      <c r="YU9" s="0"/>
+      <c r="YV9" s="0"/>
+      <c r="YW9" s="0"/>
+      <c r="YX9" s="0"/>
+      <c r="YY9" s="0"/>
+      <c r="YZ9" s="0"/>
+      <c r="ZA9" s="0"/>
+      <c r="ZB9" s="0"/>
+      <c r="ZC9" s="0"/>
+      <c r="ZD9" s="0"/>
+      <c r="ZE9" s="0"/>
+      <c r="ZF9" s="0"/>
+      <c r="ZG9" s="0"/>
+      <c r="ZH9" s="0"/>
+      <c r="ZI9" s="0"/>
+      <c r="ZJ9" s="0"/>
+      <c r="ZK9" s="0"/>
+      <c r="ZL9" s="0"/>
+      <c r="ZM9" s="0"/>
+      <c r="ZN9" s="0"/>
+      <c r="ZO9" s="0"/>
+      <c r="ZP9" s="0"/>
+      <c r="ZQ9" s="0"/>
+      <c r="ZR9" s="0"/>
+      <c r="ZS9" s="0"/>
+      <c r="ZT9" s="0"/>
+      <c r="ZU9" s="0"/>
+      <c r="ZV9" s="0"/>
+      <c r="ZW9" s="0"/>
+      <c r="ZX9" s="0"/>
+      <c r="ZY9" s="0"/>
+      <c r="ZZ9" s="0"/>
+      <c r="AAA9" s="0"/>
+      <c r="AAB9" s="0"/>
+      <c r="AAC9" s="0"/>
+      <c r="AAD9" s="0"/>
+      <c r="AAE9" s="0"/>
+      <c r="AAF9" s="0"/>
+      <c r="AAG9" s="0"/>
+      <c r="AAH9" s="0"/>
+      <c r="AAI9" s="0"/>
+      <c r="AAJ9" s="0"/>
+      <c r="AAK9" s="0"/>
+      <c r="AAL9" s="0"/>
+      <c r="AAM9" s="0"/>
+      <c r="AAN9" s="0"/>
+      <c r="AAO9" s="0"/>
+      <c r="AAP9" s="0"/>
+      <c r="AAQ9" s="0"/>
+      <c r="AAR9" s="0"/>
+      <c r="AAS9" s="0"/>
+      <c r="AAT9" s="0"/>
+      <c r="AAU9" s="0"/>
+      <c r="AAV9" s="0"/>
+      <c r="AAW9" s="0"/>
+      <c r="AAX9" s="0"/>
+      <c r="AAY9" s="0"/>
+      <c r="AAZ9" s="0"/>
+      <c r="ABA9" s="0"/>
+      <c r="ABB9" s="0"/>
+      <c r="ABC9" s="0"/>
+      <c r="ABD9" s="0"/>
+      <c r="ABE9" s="0"/>
+      <c r="ABF9" s="0"/>
+      <c r="ABG9" s="0"/>
+      <c r="ABH9" s="0"/>
+      <c r="ABI9" s="0"/>
+      <c r="ABJ9" s="0"/>
+      <c r="ABK9" s="0"/>
+      <c r="ABL9" s="0"/>
+      <c r="ABM9" s="0"/>
+      <c r="ABN9" s="0"/>
+      <c r="ABO9" s="0"/>
+      <c r="ABP9" s="0"/>
+      <c r="ABQ9" s="0"/>
+      <c r="ABR9" s="0"/>
+      <c r="ABS9" s="0"/>
+      <c r="ABT9" s="0"/>
+      <c r="ABU9" s="0"/>
+      <c r="ABV9" s="0"/>
+      <c r="ABW9" s="0"/>
+      <c r="ABX9" s="0"/>
+      <c r="ABY9" s="0"/>
+      <c r="ABZ9" s="0"/>
+      <c r="ACA9" s="0"/>
+      <c r="ACB9" s="0"/>
+      <c r="ACC9" s="0"/>
+      <c r="ACD9" s="0"/>
+      <c r="ACE9" s="0"/>
+      <c r="ACF9" s="0"/>
+      <c r="ACG9" s="0"/>
+      <c r="ACH9" s="0"/>
+      <c r="ACI9" s="0"/>
+      <c r="ACJ9" s="0"/>
+      <c r="ACK9" s="0"/>
+      <c r="ACL9" s="0"/>
+      <c r="ACM9" s="0"/>
+      <c r="ACN9" s="0"/>
+      <c r="ACO9" s="0"/>
+      <c r="ACP9" s="0"/>
+      <c r="ACQ9" s="0"/>
+      <c r="ACR9" s="0"/>
+      <c r="ACS9" s="0"/>
+      <c r="ACT9" s="0"/>
+      <c r="ACU9" s="0"/>
+      <c r="ACV9" s="0"/>
+      <c r="ACW9" s="0"/>
+      <c r="ACX9" s="0"/>
+      <c r="ACY9" s="0"/>
+      <c r="ACZ9" s="0"/>
+      <c r="ADA9" s="0"/>
+      <c r="ADB9" s="0"/>
+      <c r="ADC9" s="0"/>
+      <c r="ADD9" s="0"/>
+      <c r="ADE9" s="0"/>
+      <c r="ADF9" s="0"/>
+      <c r="ADG9" s="0"/>
+      <c r="ADH9" s="0"/>
+      <c r="ADI9" s="0"/>
+      <c r="ADJ9" s="0"/>
+      <c r="ADK9" s="0"/>
+      <c r="ADL9" s="0"/>
+      <c r="ADM9" s="0"/>
+      <c r="ADN9" s="0"/>
+      <c r="ADO9" s="0"/>
+      <c r="ADP9" s="0"/>
+      <c r="ADQ9" s="0"/>
+      <c r="ADR9" s="0"/>
+      <c r="ADS9" s="0"/>
+      <c r="ADT9" s="0"/>
+      <c r="ADU9" s="0"/>
+      <c r="ADV9" s="0"/>
+      <c r="ADW9" s="0"/>
+      <c r="ADX9" s="0"/>
+      <c r="ADY9" s="0"/>
+      <c r="ADZ9" s="0"/>
+      <c r="AEA9" s="0"/>
+      <c r="AEB9" s="0"/>
+      <c r="AEC9" s="0"/>
+      <c r="AED9" s="0"/>
+      <c r="AEE9" s="0"/>
+      <c r="AEF9" s="0"/>
+      <c r="AEG9" s="0"/>
+      <c r="AEH9" s="0"/>
+      <c r="AEI9" s="0"/>
+      <c r="AEJ9" s="0"/>
+      <c r="AEK9" s="0"/>
+      <c r="AEL9" s="0"/>
+      <c r="AEM9" s="0"/>
+      <c r="AEN9" s="0"/>
+      <c r="AEO9" s="0"/>
+      <c r="AEP9" s="0"/>
+      <c r="AEQ9" s="0"/>
+      <c r="AER9" s="0"/>
+      <c r="AES9" s="0"/>
+      <c r="AET9" s="0"/>
+      <c r="AEU9" s="0"/>
+      <c r="AEV9" s="0"/>
+      <c r="AEW9" s="0"/>
+      <c r="AEX9" s="0"/>
+      <c r="AEY9" s="0"/>
+      <c r="AEZ9" s="0"/>
+      <c r="AFA9" s="0"/>
+      <c r="AFB9" s="0"/>
+      <c r="AFC9" s="0"/>
+      <c r="AFD9" s="0"/>
+      <c r="AFE9" s="0"/>
+      <c r="AFF9" s="0"/>
+      <c r="AFG9" s="0"/>
+      <c r="AFH9" s="0"/>
+      <c r="AFI9" s="0"/>
+      <c r="AFJ9" s="0"/>
+      <c r="AFK9" s="0"/>
+      <c r="AFL9" s="0"/>
+      <c r="AFM9" s="0"/>
+      <c r="AFN9" s="0"/>
+      <c r="AFO9" s="0"/>
+      <c r="AFP9" s="0"/>
+      <c r="AFQ9" s="0"/>
+      <c r="AFR9" s="0"/>
+      <c r="AFS9" s="0"/>
+      <c r="AFT9" s="0"/>
+      <c r="AFU9" s="0"/>
+      <c r="AFV9" s="0"/>
+      <c r="AFW9" s="0"/>
+      <c r="AFX9" s="0"/>
+      <c r="AFY9" s="0"/>
+      <c r="AFZ9" s="0"/>
+      <c r="AGA9" s="0"/>
+      <c r="AGB9" s="0"/>
+      <c r="AGC9" s="0"/>
+      <c r="AGD9" s="0"/>
+      <c r="AGE9" s="0"/>
+      <c r="AGF9" s="0"/>
+      <c r="AGG9" s="0"/>
+      <c r="AGH9" s="0"/>
+      <c r="AGI9" s="0"/>
+      <c r="AGJ9" s="0"/>
+      <c r="AGK9" s="0"/>
+      <c r="AGL9" s="0"/>
+      <c r="AGM9" s="0"/>
+      <c r="AGN9" s="0"/>
+      <c r="AGO9" s="0"/>
+      <c r="AGP9" s="0"/>
+      <c r="AGQ9" s="0"/>
+      <c r="AGR9" s="0"/>
+      <c r="AGS9" s="0"/>
+      <c r="AGT9" s="0"/>
+      <c r="AGU9" s="0"/>
+      <c r="AGV9" s="0"/>
+      <c r="AGW9" s="0"/>
+      <c r="AGX9" s="0"/>
+      <c r="AGY9" s="0"/>
+      <c r="AGZ9" s="0"/>
+      <c r="AHA9" s="0"/>
+      <c r="AHB9" s="0"/>
+      <c r="AHC9" s="0"/>
+      <c r="AHD9" s="0"/>
+      <c r="AHE9" s="0"/>
+      <c r="AHF9" s="0"/>
+      <c r="AHG9" s="0"/>
+      <c r="AHH9" s="0"/>
+      <c r="AHI9" s="0"/>
+      <c r="AHJ9" s="0"/>
+      <c r="AHK9" s="0"/>
+      <c r="AHL9" s="0"/>
+      <c r="AHM9" s="0"/>
+      <c r="AHN9" s="0"/>
+      <c r="AHO9" s="0"/>
+      <c r="AHP9" s="0"/>
+      <c r="AHQ9" s="0"/>
+      <c r="AHR9" s="0"/>
+      <c r="AHS9" s="0"/>
+      <c r="AHT9" s="0"/>
+      <c r="AHU9" s="0"/>
+      <c r="AHV9" s="0"/>
+      <c r="AHW9" s="0"/>
+      <c r="AHX9" s="0"/>
+      <c r="AHY9" s="0"/>
+      <c r="AHZ9" s="0"/>
+      <c r="AIA9" s="0"/>
+      <c r="AIB9" s="0"/>
+      <c r="AIC9" s="0"/>
+      <c r="AID9" s="0"/>
+      <c r="AIE9" s="0"/>
+      <c r="AIF9" s="0"/>
+      <c r="AIG9" s="0"/>
+      <c r="AIH9" s="0"/>
+      <c r="AII9" s="0"/>
+      <c r="AIJ9" s="0"/>
+      <c r="AIK9" s="0"/>
+      <c r="AIL9" s="0"/>
+      <c r="AIM9" s="0"/>
+      <c r="AIN9" s="0"/>
+      <c r="AIO9" s="0"/>
+      <c r="AIP9" s="0"/>
+      <c r="AIQ9" s="0"/>
+      <c r="AIR9" s="0"/>
+      <c r="AIS9" s="0"/>
+      <c r="AIT9" s="0"/>
+      <c r="AIU9" s="0"/>
+      <c r="AIV9" s="0"/>
+      <c r="AIW9" s="0"/>
+      <c r="AIX9" s="0"/>
+      <c r="AIY9" s="0"/>
+      <c r="AIZ9" s="0"/>
+      <c r="AJA9" s="0"/>
+      <c r="AJB9" s="0"/>
+      <c r="AJC9" s="0"/>
+      <c r="AJD9" s="0"/>
+      <c r="AJE9" s="0"/>
+      <c r="AJF9" s="0"/>
+      <c r="AJG9" s="0"/>
+      <c r="AJH9" s="0"/>
+      <c r="AJI9" s="0"/>
+      <c r="AJJ9" s="0"/>
+      <c r="AJK9" s="0"/>
+      <c r="AJL9" s="0"/>
+      <c r="AJM9" s="0"/>
+      <c r="AJN9" s="0"/>
+      <c r="AJO9" s="0"/>
+      <c r="AJP9" s="0"/>
+      <c r="AJQ9" s="0"/>
+      <c r="AJR9" s="0"/>
+      <c r="AJS9" s="0"/>
+      <c r="AJT9" s="0"/>
+      <c r="AJU9" s="0"/>
+      <c r="AJV9" s="0"/>
+      <c r="AJW9" s="0"/>
+      <c r="AJX9" s="0"/>
+      <c r="AJY9" s="0"/>
+      <c r="AJZ9" s="0"/>
+      <c r="AKA9" s="0"/>
+      <c r="AKB9" s="0"/>
+      <c r="AKC9" s="0"/>
+      <c r="AKD9" s="0"/>
+      <c r="AKE9" s="0"/>
+      <c r="AKF9" s="0"/>
+      <c r="AKG9" s="0"/>
+      <c r="AKH9" s="0"/>
+      <c r="AKI9" s="0"/>
+      <c r="AKJ9" s="0"/>
+      <c r="AKK9" s="0"/>
+      <c r="AKL9" s="0"/>
+      <c r="AKM9" s="0"/>
+      <c r="AKN9" s="0"/>
+      <c r="AKO9" s="0"/>
+      <c r="AKP9" s="0"/>
+      <c r="AKQ9" s="0"/>
+      <c r="AKR9" s="0"/>
+      <c r="AKS9" s="0"/>
+      <c r="AKT9" s="0"/>
+      <c r="AKU9" s="0"/>
+      <c r="AKV9" s="0"/>
+      <c r="AKW9" s="0"/>
+      <c r="AKX9" s="0"/>
+      <c r="AKY9" s="0"/>
+      <c r="AKZ9" s="0"/>
+      <c r="ALA9" s="0"/>
+      <c r="ALB9" s="0"/>
+      <c r="ALC9" s="0"/>
+      <c r="ALD9" s="0"/>
+      <c r="ALE9" s="0"/>
+      <c r="ALF9" s="0"/>
+      <c r="ALG9" s="0"/>
+      <c r="ALH9" s="0"/>
+      <c r="ALI9" s="0"/>
+      <c r="ALJ9" s="0"/>
+      <c r="ALK9" s="0"/>
+      <c r="ALL9" s="0"/>
+      <c r="ALM9" s="0"/>
+      <c r="ALN9" s="0"/>
+      <c r="ALO9" s="0"/>
+      <c r="ALP9" s="0"/>
+      <c r="ALQ9" s="0"/>
+      <c r="ALR9" s="0"/>
+      <c r="ALS9" s="0"/>
+      <c r="ALT9" s="0"/>
+    </row>
+    <row r="10" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="F10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="I10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="J10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="ALU9" s="15"/>
-      <c r="ALV9" s="15"/>
-      <c r="ALW9" s="15"/>
-      <c r="ALX9" s="15"/>
-      <c r="ALY9" s="15"/>
-      <c r="ALZ9" s="15"/>
-      <c r="AMA9" s="15"/>
-      <c r="AMB9" s="15"/>
-      <c r="AMC9" s="15"/>
-      <c r="AMD9" s="15"/>
-      <c r="AME9" s="15"/>
-      <c r="AMF9" s="15"/>
-      <c r="AMG9" s="15"/>
-      <c r="AMH9" s="15"/>
-      <c r="AMI9" s="15"/>
-      <c r="AMJ9" s="15"/>
+      <c r="K10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="ALU10" s="15"/>
+      <c r="ALV10" s="15"/>
+      <c r="ALW10" s="15"/>
+      <c r="ALX10" s="15"/>
+      <c r="ALY10" s="15"/>
+      <c r="ALZ10" s="15"/>
+      <c r="AMA10" s="15"/>
+      <c r="AMB10" s="15"/>
+      <c r="AMC10" s="15"/>
+      <c r="AMD10" s="15"/>
+      <c r="AME10" s="15"/>
+      <c r="AMF10" s="15"/>
+      <c r="AMG10" s="15"/>
+      <c r="AMH10" s="15"/>
+      <c r="AMI10" s="15"/>
+      <c r="AMJ10" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[IMP] Adjust search name in building
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_before_due.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_before_due.xlsx
@@ -77,7 +77,7 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
@@ -164,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,16 +177,20 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -256,29 +260,30 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="26.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="27.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="21.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="21.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="29.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="29.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1008" min="12" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="29.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1008" min="12" style="6" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1009" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="0"/>
-      <c r="J1" s="7"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1279,18 +1284,18 @@
       <c r="ALT1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="0"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -2291,18 +2296,18 @@
       <c r="ALT2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="0"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="0"/>
-      <c r="J3" s="7"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -3303,18 +3308,18 @@
       <c r="ALT3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="0"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -4315,18 +4320,18 @@
       <c r="ALT4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="0"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
@@ -5327,18 +5332,18 @@
       <c r="ALT5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="0"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
@@ -6339,18 +6344,18 @@
       <c r="ALT6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="0"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -7355,12 +7360,12 @@
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="0"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
@@ -8360,56 +8365,56 @@
       <c r="ALS8" s="0"/>
       <c r="ALT8" s="0"/>
     </row>
-    <row r="9" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+    <row r="9" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="ALU9" s="15"/>
-      <c r="ALV9" s="15"/>
-      <c r="ALW9" s="15"/>
-      <c r="ALX9" s="15"/>
-      <c r="ALY9" s="15"/>
-      <c r="ALZ9" s="15"/>
-      <c r="AMA9" s="15"/>
-      <c r="AMB9" s="15"/>
-      <c r="AMC9" s="15"/>
-      <c r="AMD9" s="15"/>
-      <c r="AME9" s="15"/>
-      <c r="AMF9" s="15"/>
-      <c r="AMG9" s="15"/>
-      <c r="AMH9" s="15"/>
-      <c r="AMI9" s="15"/>
-      <c r="AMJ9" s="15"/>
+      <c r="ALU9" s="16"/>
+      <c r="ALV9" s="16"/>
+      <c r="ALW9" s="16"/>
+      <c r="ALX9" s="16"/>
+      <c r="ALY9" s="16"/>
+      <c r="ALZ9" s="16"/>
+      <c r="AMA9" s="16"/>
+      <c r="AMB9" s="16"/>
+      <c r="AMC9" s="16"/>
+      <c r="AMD9" s="16"/>
+      <c r="AME9" s="16"/>
+      <c r="AMF9" s="16"/>
+      <c r="AMG9" s="16"/>
+      <c r="AMH9" s="16"/>
+      <c r="AMI9" s="16"/>
+      <c r="AMJ9" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>